<commit_message>
objects added and collision completed !!!
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="E11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>hard wall</t>
   </si>
@@ -169,6 +170,21 @@
   </si>
   <si>
     <t>start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turret up </t>
+  </si>
+  <si>
+    <t>turret down</t>
+  </si>
+  <si>
+    <t>turret left</t>
+  </si>
+  <si>
+    <t>turret Right</t>
+  </si>
+  <si>
+    <t>repaire</t>
   </si>
 </sst>
 </file>
@@ -306,7 +322,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -322,6 +338,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -607,7 +626,7 @@
   <dimension ref="A1:AD27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE15" sqref="AE15"/>
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,9 +698,7 @@
       <c r="X2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="Y2" s="16"/>
       <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:29" ht="19.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -710,7 +727,9 @@
       <c r="U3" s="8"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="X3" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="6"/>
     </row>
@@ -761,9 +780,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="I5" s="17"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -784,7 +801,7 @@
       <c r="Y5" s="8"/>
       <c r="Z5" s="6"/>
       <c r="AB5" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AC5" s="3">
         <v>6</v>
@@ -801,7 +818,9 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="I6" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -931,6 +950,12 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="6"/>
+      <c r="AB9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:29" ht="19.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
@@ -963,24 +988,32 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="6"/>
+      <c r="AB10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:29" ht="19.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>15</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="12" t="s">
-        <v>8</v>
-      </c>
+      <c r="C11" s="16"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="L11" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -995,6 +1028,12 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="6"/>
+      <c r="AB11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:29" ht="19.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
@@ -1025,6 +1064,12 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="6"/>
+      <c r="AB12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:29" ht="19.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
@@ -1033,10 +1078,14 @@
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="7"/>
@@ -1057,17 +1106,21 @@
         <v>6</v>
       </c>
       <c r="Z13" s="6"/>
+      <c r="AB13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:29" ht="19.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="12" t="s">
-        <v>8</v>
-      </c>
+      <c r="C14" s="16"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1103,11 +1156,11 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="15"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1173,7 +1226,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="12" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="8"/>
@@ -1209,10 +1262,10 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="12" t="s">
+      <c r="S18" s="12" t="s">
         <v>2</v>
       </c>
+      <c r="T18" s="15"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="2"/>
@@ -1242,9 +1295,7 @@
       <c r="J19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="K19" s="15"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1257,10 +1308,10 @@
       <c r="U19" s="2"/>
       <c r="V19" s="6"/>
       <c r="W19" s="8"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="12" t="s">
+      <c r="X19" s="12" t="s">
         <v>7</v>
       </c>
+      <c r="Y19" s="15"/>
       <c r="Z19" s="6"/>
       <c r="AB19" s="5"/>
       <c r="AC19" s="3" t="s">
@@ -1284,7 +1335,9 @@
       <c r="I20" s="6"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="L20" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="8"/>
@@ -1348,20 +1401,20 @@
       <c r="A22" s="1">
         <v>4</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="10"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="12" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -1479,8 +1532,8 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
       <c r="Z25" s="6"/>
     </row>
     <row r="26" spans="1:30" ht="19.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>